<commit_message>
Latest data: for Scottish Tue May 11 17:18:31 UTC 2021
</commit_message>
<xml_diff>
--- a/uk/scotland/COVID-19%2Bdaily%2Bdata%2B-%2Bby%2BNHS%2BBoard%2B-%2B11%2BMay%2B2021.xlsx
+++ b/uk/scotland/COVID-19%2Bdaily%2Bdata%2B-%2Bby%2BNHS%2BBoard%2B-%2B11%2BMay%2B2021.xlsx
@@ -8846,10 +8846,10 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:V449"/>
+  <dimension ref="A1:V451"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B414" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B417" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight"/>
@@ -30623,7 +30623,54 @@
       </c>
     </row>
     <row r="434" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B434" s="151"/>
+      <c r="A434" s="147">
+        <v>44327</v>
+      </c>
+      <c r="B434" s="122">
+        <v>17127</v>
+      </c>
+      <c r="C434" s="122">
+        <v>2897</v>
+      </c>
+      <c r="D434" s="122">
+        <v>4208</v>
+      </c>
+      <c r="E434" s="122">
+        <v>11580</v>
+      </c>
+      <c r="F434" s="122">
+        <v>12741</v>
+      </c>
+      <c r="G434" s="122">
+        <v>15221</v>
+      </c>
+      <c r="H434" s="122">
+        <v>70597</v>
+      </c>
+      <c r="I434" s="122">
+        <v>5165</v>
+      </c>
+      <c r="J434" s="122">
+        <v>41437</v>
+      </c>
+      <c r="K434" s="122">
+        <v>31740</v>
+      </c>
+      <c r="L434" s="122">
+        <v>72</v>
+      </c>
+      <c r="M434" s="122">
+        <v>235</v>
+      </c>
+      <c r="N434" s="122">
+        <v>14764</v>
+      </c>
+      <c r="O434" s="122">
+        <v>294</v>
+      </c>
+      <c r="P434" s="123">
+        <v>228078</v>
+      </c>
     </row>
     <row r="435" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B435" s="151"/>
@@ -30637,36 +30684,54 @@
     <row r="437" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B437" s="151"/>
       <c r="I437" s="151"/>
+      <c r="J437" s="151"/>
     </row>
     <row r="438" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B438" s="151"/>
       <c r="D438" s="151"/>
       <c r="I438" s="151"/>
+      <c r="J438" s="151"/>
     </row>
     <row r="439" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I439" s="151"/>
+      <c r="J439" s="151"/>
     </row>
     <row r="440" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I440" s="151"/>
+      <c r="J440" s="151"/>
     </row>
     <row r="441" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B441" s="151"/>
       <c r="I441" s="151"/>
+      <c r="J441" s="151"/>
     </row>
     <row r="442" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I442" s="151"/>
+      <c r="J442" s="151"/>
     </row>
     <row r="443" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I443" s="151"/>
+      <c r="J443" s="151"/>
     </row>
     <row r="444" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I444" s="151"/>
+      <c r="J444" s="151"/>
+    </row>
+    <row r="445" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J445" s="151"/>
+    </row>
+    <row r="446" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J446" s="151"/>
     </row>
     <row r="447" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I447" s="151"/>
     </row>
-    <row r="449" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="449" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I449" s="151"/>
+      <c r="J449" s="151"/>
+    </row>
+    <row r="451" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="J451" s="151"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -88422,7 +88487,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2021-05-11T11:16:41Z</value>
+      <value order="0">2021-05-11T14:36:01Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -88437,13 +88502,13 @@
       <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA48520335</value>
+      <value order="0">vA48531581</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">78.74</value>
+      <value order="0">78.76</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">830</value>
+      <value order="0">832</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>